<commit_message>
Added time complexity analysis
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgaud/Downloads/CASCON 2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgaud/Downloads/CASCON2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5247D3E5-6235-014B-940F-04A5D87845F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{088E0890-D87D-4151-ABB2-A84E195285CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-67580" yWindow="-17140" windowWidth="34400" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34400" yWindow="-17140" windowWidth="34400" windowHeight="28300" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="CIC IDS 2017" sheetId="4" r:id="rId4"/>
     <sheet name="NF-UNSW-NB15-v2" sheetId="5" r:id="rId5"/>
     <sheet name="NF-CSE-CIC-IDS2018-v2" sheetId="6" r:id="rId6"/>
+    <sheet name="Time" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="50">
   <si>
     <t>Meta-classifier</t>
   </si>
@@ -61,6 +62,9 @@
     <t>w/ Threshold</t>
   </si>
   <si>
+    <t>NSLKDD</t>
+  </si>
+  <si>
     <t>No unknown</t>
   </si>
   <si>
@@ -70,9 +74,6 @@
     <t>Detection Rate</t>
   </si>
   <si>
-    <t>NSLKDD</t>
-  </si>
-  <si>
     <t>False Alarm Rate</t>
   </si>
   <si>
@@ -167,6 +168,30 @@
   </si>
   <si>
     <t>$C_5$ unknown</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Predictions</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Ratio Training</t>
+  </si>
+  <si>
+    <t>Ratio Predictions</t>
+  </si>
+  <si>
+    <t>Ratio Total</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Ratio Average</t>
   </si>
 </sst>
 </file>
@@ -176,7 +201,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +222,32 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -219,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -233,10 +284,25 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,51 +640,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView zoomScale="160" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" customWidth="1"/>
-    <col min="7" max="7" width="17.83203125" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="F2" s="14"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I2" s="14"/>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -639,13 +705,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="6" t="s">
+    <row r="4" spans="1:9">
+      <c r="A4" s="14" t="s">
         <v>6</v>
       </c>
+      <c r="B4" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3">
         <v>0.93530486822317405</v>
@@ -664,11 +732,11 @@
         <v>0.93056516190217198</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="6"/>
+    <row r="5" spans="1:9">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3">
         <v>0.99922871967465998</v>
@@ -687,11 +755,9 @@
         <v>0.99950918524750998</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="6"/>
+    <row r="6" spans="1:9">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
@@ -712,13 +778,13 @@
         <v>2.2017873332469801E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6" t="s">
+    <row r="7" spans="1:9">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" s="3">
         <v>0.52773949820049004</v>
@@ -737,11 +803,11 @@
         <v>0.65770682418169402</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
+    <row r="8" spans="1:9">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D8" s="3">
         <v>0.535214664737096</v>
@@ -760,9 +826,9 @@
         <v>0.66386878919440395</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
+    <row r="9" spans="1:9">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
@@ -783,9 +849,9 @@
         <v>1.00289725874749E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+    <row r="10" spans="1:9">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
@@ -806,13 +872,13 @@
         <v>0.172091816884969</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6" t="s">
+    <row r="11" spans="1:9">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" s="3">
         <v>0.78537740262462696</v>
@@ -831,11 +897,11 @@
         <v>0.83647628230806903</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
+    <row r="12" spans="1:9">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D12" s="3">
         <v>0.99846229118613194</v>
@@ -854,9 +920,9 @@
         <v>0.99657510309638597</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+    <row r="13" spans="1:9">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="2" t="s">
         <v>10</v>
       </c>
@@ -877,9 +943,9 @@
         <v>1.3639020588426299E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
+    <row r="14" spans="1:9">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
@@ -900,13 +966,13 @@
         <v>0.23170731707316999</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6" t="s">
+    <row r="15" spans="1:9">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D15" s="3">
         <v>0.58436337134635197</v>
@@ -925,11 +991,11 @@
         <v>0.70552012799500397</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
+    <row r="16" spans="1:9">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D16" s="3">
         <v>0.81982720565050105</v>
@@ -948,9 +1014,9 @@
         <v>0.85262029387652105</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
+    <row r="17" spans="1:9">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="2" t="s">
         <v>10</v>
       </c>
@@ -971,9 +1037,9 @@
         <v>5.7774247129342097E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
+    <row r="18" spans="1:9">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="2" t="s">
         <v>16</v>
       </c>
@@ -994,7 +1060,7 @@
         <v>0.48132444982838601</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1005,15 +1071,15 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:9">
+      <c r="A20" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>6</v>
+      <c r="B20" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D20" s="3">
         <v>0.77362613418305104</v>
@@ -1032,11 +1098,11 @@
         <v>0.78478734931818805</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
+    <row r="21" spans="1:9">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D21" s="3">
         <v>0.99995635316112197</v>
@@ -1055,9 +1121,9 @@
         <v>0.99997453934398794</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
+    <row r="22" spans="1:9">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="2" t="s">
         <v>10</v>
       </c>
@@ -1078,13 +1144,13 @@
         <v>2.9618473895582299E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6" t="s">
+    <row r="23" spans="1:9">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D23" s="3">
         <v>0.64105936504750805</v>
@@ -1103,11 +1169,11 @@
         <v>0.77960641977987899</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
+    <row r="24" spans="1:9">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
       <c r="C24" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D24" s="3">
         <v>0.99621389837535801</v>
@@ -1126,9 +1192,9 @@
         <v>0.99694856939185905</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
+    <row r="25" spans="1:9">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="2" t="s">
         <v>10</v>
       </c>
@@ -1149,9 +1215,9 @@
         <v>2.2807906741003501E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
+    <row r="26" spans="1:9">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="2" t="s">
         <v>19</v>
       </c>
@@ -1172,13 +1238,13 @@
         <v>0.84489647657101297</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6" t="s">
+    <row r="27" spans="1:9">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D27" s="3">
         <v>0.60830370596031402</v>
@@ -1197,11 +1263,11 @@
         <v>0.67232924073303402</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
+    <row r="28" spans="1:9">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
       <c r="C28" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D28" s="3">
         <v>0.99749041629992796</v>
@@ -1220,9 +1286,9 @@
         <v>0.99952354280476896</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
+    <row r="29" spans="1:9">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="2" t="s">
         <v>10</v>
       </c>
@@ -1243,9 +1309,9 @@
         <v>3.1818181818181801E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
+    <row r="30" spans="1:9">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
       <c r="C30" s="2" t="s">
         <v>21</v>
       </c>
@@ -1266,7 +1332,7 @@
         <v>0.64854614412136502</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -1274,15 +1340,15 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+    <row r="32" spans="1:9" ht="15" customHeight="1">
+      <c r="A32" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>6</v>
+      <c r="B32" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D32" s="3">
         <v>0.61270866389913503</v>
@@ -1301,11 +1367,11 @@
         <v>0.46055352513414599</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
-      <c r="B33" s="6"/>
+    <row r="33" spans="1:9">
+      <c r="A33" s="15"/>
+      <c r="B33" s="14"/>
       <c r="C33" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D33" s="3">
         <v>0.995267382882703</v>
@@ -1324,9 +1390,9 @@
         <v>0.96399616598106896</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="7"/>
-      <c r="B34" s="6"/>
+    <row r="34" spans="1:9">
+      <c r="A34" s="15"/>
+      <c r="B34" s="14"/>
       <c r="C34" s="2" t="s">
         <v>10</v>
       </c>
@@ -1347,13 +1413,13 @@
         <v>0.12505009141683501</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="7"/>
-      <c r="B35" s="6" t="s">
+    <row r="35" spans="1:9">
+      <c r="A35" s="15"/>
+      <c r="B35" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D35" s="3">
         <v>0.484797234226718</v>
@@ -1372,11 +1438,11 @@
         <v>0.46284235599633999</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="7"/>
-      <c r="B36" s="6"/>
+    <row r="36" spans="1:9">
+      <c r="A36" s="15"/>
+      <c r="B36" s="14"/>
       <c r="C36" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D36" s="3">
         <v>0.84992904612704201</v>
@@ -1395,9 +1461,9 @@
         <v>0.98127098759360998</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="7"/>
-      <c r="B37" s="6"/>
+    <row r="37" spans="1:9">
+      <c r="A37" s="15"/>
+      <c r="B37" s="14"/>
       <c r="C37" s="2" t="s">
         <v>10</v>
       </c>
@@ -1418,9 +1484,9 @@
         <v>6.5253619790351505E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="7"/>
-      <c r="B38" s="6"/>
+    <row r="38" spans="1:9">
+      <c r="A38" s="15"/>
+      <c r="B38" s="14"/>
       <c r="C38" s="2" t="s">
         <v>24</v>
       </c>
@@ -1441,13 +1507,13 @@
         <v>2.5542671545934099E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="7"/>
-      <c r="B39" s="6" t="s">
+    <row r="39" spans="1:9">
+      <c r="A39" s="15"/>
+      <c r="B39" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D39" s="3">
         <v>0.74625207729501097</v>
@@ -1466,11 +1532,11 @@
         <v>0.76664547927022897</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="7"/>
-      <c r="B40" s="6"/>
+    <row r="40" spans="1:9">
+      <c r="A40" s="15"/>
+      <c r="B40" s="14"/>
       <c r="C40" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D40" s="3">
         <v>0.96803711186520403</v>
@@ -1489,9 +1555,9 @@
         <v>0.99014338675192703</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="7"/>
-      <c r="B41" s="6"/>
+    <row r="41" spans="1:9">
+      <c r="A41" s="15"/>
+      <c r="B41" s="14"/>
       <c r="C41" s="2" t="s">
         <v>10</v>
       </c>
@@ -1512,9 +1578,9 @@
         <v>1.6211706180535801E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="7"/>
-      <c r="B42" s="6"/>
+    <row r="42" spans="1:9">
+      <c r="A42" s="15"/>
+      <c r="B42" s="14"/>
       <c r="C42" s="2" t="s">
         <v>26</v>
       </c>
@@ -1535,13 +1601,13 @@
         <v>0.56436719174361705</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="7"/>
-      <c r="B43" s="6" t="s">
+    <row r="43" spans="1:9">
+      <c r="A43" s="15"/>
+      <c r="B43" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D43" s="3">
         <v>0.60404147069907599</v>
@@ -1560,11 +1626,11 @@
         <v>0.60995753367927596</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="7"/>
-      <c r="B44" s="6"/>
+    <row r="44" spans="1:9">
+      <c r="A44" s="15"/>
+      <c r="B44" s="14"/>
       <c r="C44" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D44" s="3">
         <v>0.99536020754340404</v>
@@ -1583,9 +1649,9 @@
         <v>0.99282578327679105</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="7"/>
-      <c r="B45" s="6"/>
+    <row r="45" spans="1:9">
+      <c r="A45" s="15"/>
+      <c r="B45" s="14"/>
       <c r="C45" s="2" t="s">
         <v>10</v>
       </c>
@@ -1606,9 +1672,9 @@
         <v>7.2343370324907896E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="7"/>
-      <c r="B46" s="6"/>
+    <row r="46" spans="1:9">
+      <c r="A46" s="15"/>
+      <c r="B46" s="14"/>
       <c r="C46" s="2" t="s">
         <v>28</v>
       </c>
@@ -1629,7 +1695,7 @@
         <v>1.00150225338007E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9">
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -1637,15 +1703,15 @@
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="7" t="s">
+    <row r="48" spans="1:9">
+      <c r="A48" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>6</v>
+      <c r="B48" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D48" s="3">
         <v>0.66839455215063803</v>
@@ -1664,11 +1730,11 @@
         <v>0.62629822314037797</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="7"/>
-      <c r="B49" s="6"/>
+    <row r="49" spans="1:9">
+      <c r="A49" s="15"/>
+      <c r="B49" s="14"/>
       <c r="C49" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D49" s="3">
         <v>0.99431907842827805</v>
@@ -1687,9 +1753,9 @@
         <v>0.99673873020882597</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="7"/>
-      <c r="B50" s="6"/>
+    <row r="50" spans="1:9">
+      <c r="A50" s="15"/>
+      <c r="B50" s="14"/>
       <c r="C50" s="2" t="s">
         <v>10</v>
       </c>
@@ -1710,13 +1776,13 @@
         <v>4.5442266972229202E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="7"/>
-      <c r="B51" s="6" t="s">
+    <row r="51" spans="1:9">
+      <c r="A51" s="15"/>
+      <c r="B51" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D51" s="3">
         <v>0.46552959800300803</v>
@@ -1735,11 +1801,11 @@
         <v>0.48865496093334798</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="7"/>
-      <c r="B52" s="6"/>
+    <row r="52" spans="1:9">
+      <c r="A52" s="15"/>
+      <c r="B52" s="14"/>
       <c r="C52" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D52" s="3">
         <v>0.830043997485858</v>
@@ -1758,9 +1824,9 @@
         <v>0.99754871150219904</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="7"/>
-      <c r="B53" s="6"/>
+    <row r="53" spans="1:9">
+      <c r="A53" s="15"/>
+      <c r="B53" s="14"/>
       <c r="C53" s="2" t="s">
         <v>10</v>
       </c>
@@ -1781,9 +1847,9 @@
         <v>0.11085414635786001</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="7"/>
-      <c r="B54" s="6"/>
+    <row r="54" spans="1:9">
+      <c r="A54" s="15"/>
+      <c r="B54" s="14"/>
       <c r="C54" s="2" t="s">
         <v>24</v>
       </c>
@@ -1804,13 +1870,13 @@
         <v>0.61091083874068697</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="7"/>
-      <c r="B55" s="6" t="s">
+    <row r="55" spans="1:9">
+      <c r="A55" s="15"/>
+      <c r="B55" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D55" s="3">
         <v>0.581928603152293</v>
@@ -1829,11 +1895,11 @@
         <v>0.65646084350151701</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="7"/>
-      <c r="B56" s="6"/>
+    <row r="56" spans="1:9">
+      <c r="A56" s="15"/>
+      <c r="B56" s="14"/>
       <c r="C56" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D56" s="3">
         <v>0.98836912065439597</v>
@@ -1852,9 +1918,9 @@
         <v>0.99377982276755195</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="7"/>
-      <c r="B57" s="6"/>
+    <row r="57" spans="1:9">
+      <c r="A57" s="15"/>
+      <c r="B57" s="14"/>
       <c r="C57" s="2" t="s">
         <v>10</v>
       </c>
@@ -1875,9 +1941,9 @@
         <v>4.3160434948073204E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="7"/>
-      <c r="B58" s="6"/>
+    <row r="58" spans="1:9">
+      <c r="A58" s="15"/>
+      <c r="B58" s="14"/>
       <c r="C58" s="2" t="s">
         <v>14</v>
       </c>
@@ -1898,13 +1964,13 @@
         <v>0.52186273182618104</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="7"/>
-      <c r="B59" s="6" t="s">
+    <row r="59" spans="1:9">
+      <c r="A59" s="15"/>
+      <c r="B59" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D59" s="3">
         <v>0.56144237783622197</v>
@@ -1923,11 +1989,11 @@
         <v>0.56949414490039896</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="7"/>
-      <c r="B60" s="6"/>
+    <row r="60" spans="1:9">
+      <c r="A60" s="15"/>
+      <c r="B60" s="14"/>
       <c r="C60" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D60" s="3">
         <v>0.99443007758106206</v>
@@ -1946,9 +2012,9 @@
         <v>0.997065844440023</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="7"/>
-      <c r="B61" s="6"/>
+    <row r="61" spans="1:9">
+      <c r="A61" s="15"/>
+      <c r="B61" s="14"/>
       <c r="C61" s="2" t="s">
         <v>10</v>
       </c>
@@ -1969,9 +2035,9 @@
         <v>4.4655822617027698E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="7"/>
-      <c r="B62" s="6"/>
+    <row r="62" spans="1:9">
+      <c r="A62" s="15"/>
+      <c r="B62" s="14"/>
       <c r="C62" s="2" t="s">
         <v>26</v>
       </c>
@@ -1992,15 +2058,15 @@
         <v>0.27065775452872198</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="7" t="s">
+    <row r="64" spans="1:9" ht="15" customHeight="1">
+      <c r="A64" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B64" s="6" t="s">
-        <v>6</v>
+      <c r="B64" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D64" s="3">
         <v>0.62959788506155301</v>
@@ -2019,11 +2085,11 @@
         <v>0.470751734583854</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" s="7"/>
-      <c r="B65" s="6"/>
+    <row r="65" spans="1:9">
+      <c r="A65" s="15"/>
+      <c r="B65" s="14"/>
       <c r="C65" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D65" s="3">
         <v>0.95248523120798501</v>
@@ -2042,9 +2108,9 @@
         <v>0.92998441194965697</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" s="7"/>
-      <c r="B66" s="6"/>
+    <row r="66" spans="1:9">
+      <c r="A66" s="15"/>
+      <c r="B66" s="14"/>
       <c r="C66" s="2" t="s">
         <v>10</v>
       </c>
@@ -2065,13 +2131,13 @@
         <v>0.55800883288038805</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="7"/>
-      <c r="B67" s="6" t="s">
+    <row r="67" spans="1:9">
+      <c r="A67" s="15"/>
+      <c r="B67" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D67" s="3">
         <v>0.68150444185321502</v>
@@ -2090,11 +2156,11 @@
         <v>0.41884552027899302</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" s="7"/>
-      <c r="B68" s="6"/>
+    <row r="68" spans="1:9">
+      <c r="A68" s="15"/>
+      <c r="B68" s="14"/>
       <c r="C68" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D68" s="3">
         <v>0.76088328193836696</v>
@@ -2113,9 +2179,9 @@
         <v>0.78536188983690203</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" s="7"/>
-      <c r="B69" s="6"/>
+    <row r="69" spans="1:9">
+      <c r="A69" s="15"/>
+      <c r="B69" s="14"/>
       <c r="C69" s="2" t="s">
         <v>10</v>
       </c>
@@ -2136,9 +2202,9 @@
         <v>0.172123404639585</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70" s="7"/>
-      <c r="B70" s="6"/>
+    <row r="70" spans="1:9">
+      <c r="A70" s="15"/>
+      <c r="B70" s="14"/>
       <c r="C70" s="2" t="s">
         <v>32</v>
       </c>
@@ -2159,13 +2225,13 @@
         <v>7.5743672733946102E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" s="7"/>
-      <c r="B71" s="6" t="s">
+    <row r="71" spans="1:9">
+      <c r="A71" s="15"/>
+      <c r="B71" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D71" s="3">
         <v>0.46711000098795202</v>
@@ -2184,11 +2250,11 @@
         <v>0.58156439779303504</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A72" s="7"/>
-      <c r="B72" s="6"/>
+    <row r="72" spans="1:9">
+      <c r="A72" s="15"/>
+      <c r="B72" s="14"/>
       <c r="C72" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D72" s="3">
         <v>0.94697820905686003</v>
@@ -2207,9 +2273,9 @@
         <v>0.99077502553626096</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A73" s="7"/>
-      <c r="B73" s="6"/>
+    <row r="73" spans="1:9">
+      <c r="A73" s="15"/>
+      <c r="B73" s="14"/>
       <c r="C73" s="2" t="s">
         <v>10</v>
       </c>
@@ -2230,9 +2296,9 @@
         <v>0.54051955650681704</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A74" s="7"/>
-      <c r="B74" s="6"/>
+    <row r="74" spans="1:9">
+      <c r="A74" s="15"/>
+      <c r="B74" s="14"/>
       <c r="C74" s="2" t="s">
         <v>16</v>
       </c>
@@ -2252,55 +2318,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9">
       <c r="A75" s="5"/>
-      <c r="B75" s="6"/>
+      <c r="B75" s="14"/>
       <c r="C75" s="2"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9">
       <c r="A76" s="5"/>
-      <c r="B76" s="6"/>
+      <c r="B76" s="14"/>
       <c r="C76" s="2"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9">
       <c r="A77" s="5"/>
-      <c r="B77" s="6"/>
+      <c r="B77" s="14"/>
       <c r="C77" s="2"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9">
       <c r="A78" s="5"/>
-      <c r="B78" s="6"/>
+      <c r="B78" s="14"/>
       <c r="C78" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="A32:A46"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="A20:A30"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="A6:A18"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="A64:A74"/>
+    <mergeCell ref="A48:A62"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="B59:B62"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="B11:B14"/>
     <mergeCell ref="B15:B18"/>
     <mergeCell ref="B4:B6"/>
-    <mergeCell ref="A48:A62"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="B71:B74"/>
-    <mergeCell ref="B75:B78"/>
-    <mergeCell ref="A64:A74"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="A20:A30"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="A4:A18"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="A32:A46"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:I5 D7:I8 D10:I12 D14:I16 D18:I21 D23:I24 D26:I28 D30:I33 D35:I36 D38:I40 D42:I44 D46:I49 D51:I52 D54:I56 D58:I60 D62:I65 D67:I68 D70:I72 D74:I74">
     <cfRule type="colorScale" priority="2">
@@ -2338,13 +2404,13 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -2356,9 +2422,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3">
         <v>0.93530486822317405</v>
@@ -2370,7 +2436,7 @@
         <v>0.93974125380018902</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
@@ -2384,7 +2450,7 @@
         <v>0.63048640527098299</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>34</v>
       </c>
@@ -2398,7 +2464,7 @@
         <v>0.83365701231505096</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>35</v>
       </c>
@@ -2412,18 +2478,18 @@
         <v>0.69429540667075296</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:4">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -2453,12 +2519,12 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -2470,9 +2536,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3">
         <v>0.77362613418305104</v>
@@ -2484,7 +2550,7 @@
         <v>0.78543896207217501</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
@@ -2498,7 +2564,7 @@
         <v>0.77887052040695104</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
@@ -2537,12 +2603,12 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
@@ -2553,9 +2619,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3">
         <v>0.61270866389913503</v>
@@ -2567,7 +2633,7 @@
         <v>0.98659510946005102</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>38</v>
       </c>
@@ -2581,7 +2647,7 @@
         <v>0.78357645036113199</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
@@ -2595,7 +2661,7 @@
         <v>0.94046140712959103</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
@@ -2634,13 +2700,13 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
@@ -2651,9 +2717,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3">
         <v>0.66839455215063803</v>
@@ -2665,7 +2731,7 @@
         <v>0.63204602231211304</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>38</v>
       </c>
@@ -2679,7 +2745,7 @@
         <v>0.55269685758461895</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>34</v>
       </c>
@@ -2693,7 +2759,7 @@
         <v>0.66103809475951403</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>39</v>
       </c>
@@ -2732,12 +2798,12 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
@@ -2748,9 +2814,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3">
         <v>0.62959788506155301</v>
@@ -2762,7 +2828,7 @@
         <v>0.79064639032981698</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
@@ -2776,7 +2842,7 @@
         <v>0.66524673305219995</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>35</v>
       </c>
@@ -2805,4 +2871,1827 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF53C2C1-6572-CB49-9175-6508079FE50B}">
+  <dimension ref="A1:V34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.28515625" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" customWidth="1"/>
+    <col min="16" max="17" width="12.140625" customWidth="1"/>
+    <col min="18" max="18" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" customWidth="1"/>
+    <col min="20" max="21" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.140625" customWidth="1"/>
+    <col min="23" max="24" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="2"/>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+    </row>
+    <row r="3" spans="1:22" ht="17.100000000000001" customHeight="1">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="2"/>
+    </row>
+    <row r="4" spans="1:22" ht="17.100000000000001" customHeight="1">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="15.75">
+      <c r="A5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="8">
+        <v>2.4812853336334202</v>
+      </c>
+      <c r="D5" s="8">
+        <f>E5-C5</f>
+        <v>0.2536258697509699</v>
+      </c>
+      <c r="E5" s="8">
+        <v>2.7349112033843901</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8">
+        <v>4.0216176509857098</v>
+      </c>
+      <c r="H5" s="8">
+        <f>G5/C5</f>
+        <v>1.6207800031996864</v>
+      </c>
+      <c r="I5" s="8">
+        <f>K5-G5</f>
+        <v>0.33279609680176048</v>
+      </c>
+      <c r="J5" s="8">
+        <f>I5/D5</f>
+        <v>1.3121535950907777</v>
+      </c>
+      <c r="K5" s="8">
+        <v>4.3544137477874703</v>
+      </c>
+      <c r="L5" s="8">
+        <f>K5/E5</f>
+        <v>1.5921590954759273</v>
+      </c>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8">
+        <v>4.4793457984924299</v>
+      </c>
+      <c r="O5" s="8">
+        <f>N5/C5</f>
+        <v>1.8052521964224042</v>
+      </c>
+      <c r="P5" s="8">
+        <f>R5-N5</f>
+        <v>0.33417010307312012</v>
+      </c>
+      <c r="Q5" s="8">
+        <f>P5/D5</f>
+        <v>1.3175710482579517</v>
+      </c>
+      <c r="R5" s="8">
+        <v>4.81351590156555</v>
+      </c>
+      <c r="S5" s="8">
+        <f>R5/E5</f>
+        <v>1.7600263934013411</v>
+      </c>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+    </row>
+    <row r="6" spans="1:22" ht="15.75">
+      <c r="A6" s="14"/>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1.9109296798705999</v>
+      </c>
+      <c r="D6" s="8">
+        <f t="shared" ref="D6:D30" si="0">E6-C6</f>
+        <v>0.22025990486144997</v>
+      </c>
+      <c r="E6" s="8">
+        <v>2.1311895847320499</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8">
+        <v>3.1080663204193102</v>
+      </c>
+      <c r="H6" s="8">
+        <f t="shared" ref="H6:H30" si="1">G6/C6</f>
+        <v>1.6264681809901949</v>
+      </c>
+      <c r="I6" s="8">
+        <f t="shared" ref="I6:I30" si="2">K6-G6</f>
+        <v>0.29014992713928001</v>
+      </c>
+      <c r="J6" s="8">
+        <f t="shared" ref="J6:J30" si="3">I6/D6</f>
+        <v>1.3173070574137991</v>
+      </c>
+      <c r="K6" s="8">
+        <v>3.3982162475585902</v>
+      </c>
+      <c r="L6" s="8">
+        <f t="shared" ref="L6:L30" si="4">K6/E6</f>
+        <v>1.5945161668880063</v>
+      </c>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8">
+        <v>3.44744420051574</v>
+      </c>
+      <c r="O6" s="8">
+        <f t="shared" ref="O6:O30" si="5">N6/C6</f>
+        <v>1.8040664901647172</v>
+      </c>
+      <c r="P6" s="8">
+        <f t="shared" ref="P6:P30" si="6">R6-N6</f>
+        <v>0.30519795417786</v>
+      </c>
+      <c r="Q6" s="8">
+        <f t="shared" ref="Q6:Q31" si="7">P6/D6</f>
+        <v>1.3856264687385504</v>
+      </c>
+      <c r="R6" s="8">
+        <v>3.7526421546936</v>
+      </c>
+      <c r="S6" s="8">
+        <f t="shared" ref="S6:S30" si="8">R6/E6</f>
+        <v>1.7608204270411785</v>
+      </c>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+    </row>
+    <row r="7" spans="1:22" ht="15.75">
+      <c r="A7" s="14"/>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1.86661720275878</v>
+      </c>
+      <c r="D7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.24370861053466997</v>
+      </c>
+      <c r="E7" s="8">
+        <v>2.1103258132934499</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8">
+        <v>3.0935575962066602</v>
+      </c>
+      <c r="H7" s="8">
+        <f t="shared" si="1"/>
+        <v>1.6573069141517152</v>
+      </c>
+      <c r="I7" s="8">
+        <f t="shared" si="2"/>
+        <v>0.31392979621886985</v>
+      </c>
+      <c r="J7" s="8">
+        <f t="shared" si="3"/>
+        <v>1.2881358419390365</v>
+      </c>
+      <c r="K7" s="8">
+        <v>3.40748739242553</v>
+      </c>
+      <c r="L7" s="8">
+        <f t="shared" si="4"/>
+        <v>1.6146736067771845</v>
+      </c>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8">
+        <v>3.39155793190002</v>
+      </c>
+      <c r="O7" s="8">
+        <f t="shared" si="5"/>
+        <v>1.8169541815469412</v>
+      </c>
+      <c r="P7" s="8">
+        <f t="shared" si="6"/>
+        <v>0.31155395507812012</v>
+      </c>
+      <c r="Q7" s="8">
+        <f t="shared" si="7"/>
+        <v>1.2783871460044227</v>
+      </c>
+      <c r="R7" s="8">
+        <v>3.7031118869781401</v>
+      </c>
+      <c r="S7" s="8">
+        <f t="shared" si="8"/>
+        <v>1.7547583712672932</v>
+      </c>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+    </row>
+    <row r="8" spans="1:22" ht="15.75">
+      <c r="A8" s="14"/>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1.86109614372253</v>
+      </c>
+      <c r="D8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.25879406929016002</v>
+      </c>
+      <c r="E8" s="8">
+        <v>2.11989021301269</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8">
+        <v>3.10674953460693</v>
+      </c>
+      <c r="H8" s="8">
+        <f t="shared" si="1"/>
+        <v>1.6693116823039928</v>
+      </c>
+      <c r="I8" s="8">
+        <f t="shared" si="2"/>
+        <v>0.32358860969543013</v>
+      </c>
+      <c r="J8" s="8">
+        <f t="shared" si="3"/>
+        <v>1.2503710405072013</v>
+      </c>
+      <c r="K8" s="8">
+        <v>3.4303381443023602</v>
+      </c>
+      <c r="L8" s="8">
+        <f t="shared" si="4"/>
+        <v>1.618167829279858</v>
+      </c>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8">
+        <v>3.6906051635742099</v>
+      </c>
+      <c r="O8" s="8">
+        <f t="shared" si="5"/>
+        <v>1.983027677545089</v>
+      </c>
+      <c r="P8" s="8">
+        <f t="shared" si="6"/>
+        <v>0.32345414161683017</v>
+      </c>
+      <c r="Q8" s="8">
+        <f t="shared" si="7"/>
+        <v>1.2498514456070213</v>
+      </c>
+      <c r="R8" s="8">
+        <v>4.01405930519104</v>
+      </c>
+      <c r="S8" s="8">
+        <f t="shared" si="8"/>
+        <v>1.893522259101543</v>
+      </c>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+    </row>
+    <row r="9" spans="1:22" s="11" customFormat="1" ht="15.75">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="10">
+        <f>AVERAGE(C5:C8)</f>
+        <v>2.0299820899963326</v>
+      </c>
+      <c r="D9" s="10">
+        <f t="shared" ref="D9:S9" si="9">AVERAGE(D5:D8)</f>
+        <v>0.24409711360931247</v>
+      </c>
+      <c r="E9" s="10">
+        <f t="shared" si="9"/>
+        <v>2.2740792036056448</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10">
+        <f t="shared" si="9"/>
+        <v>3.3324977755546525</v>
+      </c>
+      <c r="H9" s="12">
+        <f>G9/C9</f>
+        <v>1.6416390036035604</v>
+      </c>
+      <c r="I9" s="10">
+        <f t="shared" si="9"/>
+        <v>0.31511610746383512</v>
+      </c>
+      <c r="J9" s="12">
+        <f>I9/D9</f>
+        <v>1.2909456519350389</v>
+      </c>
+      <c r="K9" s="10">
+        <f t="shared" si="9"/>
+        <v>3.6476138830184874</v>
+      </c>
+      <c r="L9" s="12">
+        <f>K9/E9</f>
+        <v>1.6039959721873573</v>
+      </c>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10">
+        <f t="shared" si="9"/>
+        <v>3.7522382736205997</v>
+      </c>
+      <c r="O9" s="12">
+        <f>N9/C9</f>
+        <v>1.8484095461292362</v>
+      </c>
+      <c r="P9" s="10">
+        <f t="shared" si="9"/>
+        <v>0.3185940384864826</v>
+      </c>
+      <c r="Q9" s="12">
+        <f>P9/D9</f>
+        <v>1.3051937967460179</v>
+      </c>
+      <c r="R9" s="10">
+        <f>AVERAGE(R5:R8)</f>
+        <v>4.0708323121070826</v>
+      </c>
+      <c r="S9" s="12">
+        <f>R9/E9</f>
+        <v>1.7901013762636819</v>
+      </c>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+    </row>
+    <row r="10" spans="1:22" ht="15.75">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+    </row>
+    <row r="11" spans="1:22" ht="15.75">
+      <c r="A11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="8">
+        <v>68.944602966308594</v>
+      </c>
+      <c r="D11" s="8">
+        <f t="shared" si="0"/>
+        <v>5.6359872817993022</v>
+      </c>
+      <c r="E11" s="8">
+        <v>74.580590248107896</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8">
+        <v>87.447476863860999</v>
+      </c>
+      <c r="H11" s="8">
+        <f>G11/C11</f>
+        <v>1.2683730575197347</v>
+      </c>
+      <c r="I11" s="8">
+        <f t="shared" si="2"/>
+        <v>6.4040923118592019</v>
+      </c>
+      <c r="J11" s="8">
+        <f>I11/D11</f>
+        <v>1.1362857990365585</v>
+      </c>
+      <c r="K11" s="8">
+        <v>93.851569175720201</v>
+      </c>
+      <c r="L11" s="8">
+        <f>K11/E11</f>
+        <v>1.2583913436928211</v>
+      </c>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8">
+        <v>115.544673204422</v>
+      </c>
+      <c r="O11" s="8">
+        <f>N11/C11</f>
+        <v>1.675905991668204</v>
+      </c>
+      <c r="P11" s="8">
+        <f t="shared" si="6"/>
+        <v>6.5638353824610078</v>
+      </c>
+      <c r="Q11" s="8">
+        <f>P11/D11</f>
+        <v>1.1646292041250823</v>
+      </c>
+      <c r="R11" s="8">
+        <v>122.108508586883</v>
+      </c>
+      <c r="S11" s="8">
+        <f>R11/E11</f>
+        <v>1.6372692704718959</v>
+      </c>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+    </row>
+    <row r="12" spans="1:22" ht="15.75">
+      <c r="A12" s="14"/>
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="8">
+        <v>55.224092960357602</v>
+      </c>
+      <c r="D12" s="8">
+        <f t="shared" si="0"/>
+        <v>5.287100791931195</v>
+      </c>
+      <c r="E12" s="8">
+        <v>60.511193752288797</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8">
+        <v>68.528267145156804</v>
+      </c>
+      <c r="H12" s="8">
+        <f>G12/C12</f>
+        <v>1.2409124979988273</v>
+      </c>
+      <c r="I12" s="8">
+        <f t="shared" si="2"/>
+        <v>5.9033427238464924</v>
+      </c>
+      <c r="J12" s="8">
+        <f>I12/D12</f>
+        <v>1.1165557374763431</v>
+      </c>
+      <c r="K12" s="8">
+        <v>74.431609869003296</v>
+      </c>
+      <c r="L12" s="8">
+        <f>K12/E12</f>
+        <v>1.2300469591411418</v>
+      </c>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8">
+        <v>89.345082759857107</v>
+      </c>
+      <c r="O12" s="8">
+        <f>N12/C12</f>
+        <v>1.6178641960492339</v>
+      </c>
+      <c r="P12" s="8">
+        <f t="shared" si="6"/>
+        <v>6.2095193862914897</v>
+      </c>
+      <c r="Q12" s="8">
+        <f>P12/D12</f>
+        <v>1.1744658614732719</v>
+      </c>
+      <c r="R12" s="8">
+        <v>95.554602146148596</v>
+      </c>
+      <c r="S12" s="8">
+        <f>R12/E12</f>
+        <v>1.5791227411132391</v>
+      </c>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+    </row>
+    <row r="13" spans="1:22" ht="15.75">
+      <c r="A13" s="14"/>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="8">
+        <v>69.742317438125596</v>
+      </c>
+      <c r="D13" s="8">
+        <f t="shared" si="0"/>
+        <v>5.5050384998321107</v>
+      </c>
+      <c r="E13" s="8">
+        <v>75.247355937957707</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8">
+        <v>81.360312461852999</v>
+      </c>
+      <c r="H13" s="8">
+        <f>G13/C13</f>
+        <v>1.1665845852345633</v>
+      </c>
+      <c r="I13" s="8">
+        <f t="shared" si="2"/>
+        <v>6.0546925067901043</v>
+      </c>
+      <c r="J13" s="8">
+        <f>I13/D13</f>
+        <v>1.0998456245083039</v>
+      </c>
+      <c r="K13" s="8">
+        <v>87.415004968643103</v>
+      </c>
+      <c r="L13" s="8">
+        <f>K13/E13</f>
+        <v>1.1617020143633718</v>
+      </c>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8">
+        <v>100.91805720329199</v>
+      </c>
+      <c r="O13" s="8">
+        <f>N13/C13</f>
+        <v>1.4470132469117487</v>
+      </c>
+      <c r="P13" s="8">
+        <f t="shared" si="6"/>
+        <v>5.9170715808870114</v>
+      </c>
+      <c r="Q13" s="8">
+        <f>P13/D13</f>
+        <v>1.0748465394142959</v>
+      </c>
+      <c r="R13" s="8">
+        <v>106.83512878417901</v>
+      </c>
+      <c r="S13" s="8">
+        <f>R13/E13</f>
+        <v>1.4197858177537264</v>
+      </c>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+    </row>
+    <row r="14" spans="1:22" s="11" customFormat="1" ht="15.75">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="10">
+        <f>AVERAGE(C11:C13)</f>
+        <v>64.637004454930604</v>
+      </c>
+      <c r="D14" s="10">
+        <f t="shared" ref="D14:S14" si="10">AVERAGE(D11:D13)</f>
+        <v>5.4760421911875357</v>
+      </c>
+      <c r="E14" s="10">
+        <f t="shared" si="10"/>
+        <v>70.113046646118136</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10">
+        <f t="shared" si="10"/>
+        <v>79.1120188236236</v>
+      </c>
+      <c r="H14" s="12">
+        <f>G14/C14</f>
+        <v>1.2239431497600726</v>
+      </c>
+      <c r="I14" s="10">
+        <f t="shared" si="10"/>
+        <v>6.1207091808319332</v>
+      </c>
+      <c r="J14" s="12">
+        <f>I14/D14</f>
+        <v>1.1177249858815632</v>
+      </c>
+      <c r="K14" s="10">
+        <f t="shared" si="10"/>
+        <v>85.232728004455538</v>
+      </c>
+      <c r="L14" s="12">
+        <f>K14/E14</f>
+        <v>1.2156471880996846</v>
+      </c>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10">
+        <f t="shared" si="10"/>
+        <v>101.9359377225237</v>
+      </c>
+      <c r="O14" s="12">
+        <f>N14/C14</f>
+        <v>1.5770523182831051</v>
+      </c>
+      <c r="P14" s="10">
+        <f t="shared" si="10"/>
+        <v>6.230142116546503</v>
+      </c>
+      <c r="Q14" s="12">
+        <f>P14/D14</f>
+        <v>1.1377089326617174</v>
+      </c>
+      <c r="R14" s="10">
+        <f>AVERAGE(R11:R13)</f>
+        <v>108.16607983907021</v>
+      </c>
+      <c r="S14" s="12">
+        <f>R14/E14</f>
+        <v>1.5427382636075893</v>
+      </c>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+    </row>
+    <row r="15" spans="1:22" ht="15.75">
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+    </row>
+    <row r="16" spans="1:22" ht="15" customHeight="1">
+      <c r="A16" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="8">
+        <v>135.70377540588299</v>
+      </c>
+      <c r="D16" s="8">
+        <f t="shared" si="0"/>
+        <v>9.3208110332490151</v>
+      </c>
+      <c r="E16" s="8">
+        <v>145.02458643913201</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8">
+        <v>159.17687010764999</v>
+      </c>
+      <c r="H16" s="8">
+        <f>G16/C16</f>
+        <v>1.1729730409604315</v>
+      </c>
+      <c r="I16" s="8">
+        <f t="shared" si="2"/>
+        <v>10.549807548523006</v>
+      </c>
+      <c r="J16" s="8">
+        <f>I16/D16</f>
+        <v>1.1318551047639458</v>
+      </c>
+      <c r="K16" s="8">
+        <v>169.726677656173</v>
+      </c>
+      <c r="L16" s="8">
+        <f>K16/E16</f>
+        <v>1.1703303682745454</v>
+      </c>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8">
+        <v>193.680277824401</v>
+      </c>
+      <c r="O16" s="8">
+        <f>N16/C16</f>
+        <v>1.4272283674136057</v>
+      </c>
+      <c r="P16" s="8">
+        <f t="shared" si="6"/>
+        <v>10.097243309020996</v>
+      </c>
+      <c r="Q16" s="8">
+        <f>P16/D16</f>
+        <v>1.0833009351871106</v>
+      </c>
+      <c r="R16" s="8">
+        <v>203.777521133422</v>
+      </c>
+      <c r="S16" s="8">
+        <f>R16/E16</f>
+        <v>1.4051239595773581</v>
+      </c>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+    </row>
+    <row r="17" spans="1:21" ht="15.75">
+      <c r="A17" s="15"/>
+      <c r="B17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="8">
+        <v>100.895361185073</v>
+      </c>
+      <c r="D17" s="8">
+        <f t="shared" si="0"/>
+        <v>8.6264979839330067</v>
+      </c>
+      <c r="E17" s="8">
+        <v>109.52185916900601</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8">
+        <v>125.89421129226599</v>
+      </c>
+      <c r="H17" s="8">
+        <f>G17/C17</f>
+        <v>1.247770064089839</v>
+      </c>
+      <c r="I17" s="8">
+        <f t="shared" si="2"/>
+        <v>9.4752395153050202</v>
+      </c>
+      <c r="J17" s="8">
+        <f>I17/D17</f>
+        <v>1.0983877273202647</v>
+      </c>
+      <c r="K17" s="8">
+        <v>135.36945080757101</v>
+      </c>
+      <c r="L17" s="8">
+        <f>K17/E17</f>
+        <v>1.2360039524044137</v>
+      </c>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8">
+        <v>152.16694474220199</v>
+      </c>
+      <c r="O17" s="8">
+        <f>N17/C17</f>
+        <v>1.5081659152107221</v>
+      </c>
+      <c r="P17" s="8">
+        <f t="shared" si="6"/>
+        <v>9.4800007343289963</v>
+      </c>
+      <c r="Q17" s="8">
+        <f>P17/D17</f>
+        <v>1.0989396568556153</v>
+      </c>
+      <c r="R17" s="8">
+        <v>161.64694547653099</v>
+      </c>
+      <c r="S17" s="8">
+        <f>R17/E17</f>
+        <v>1.4759331762903094</v>
+      </c>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+    </row>
+    <row r="18" spans="1:21" ht="15.75">
+      <c r="A18" s="15"/>
+      <c r="B18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="8">
+        <v>109.462527990341</v>
+      </c>
+      <c r="D18" s="8">
+        <f t="shared" si="0"/>
+        <v>8.4035699367519925</v>
+      </c>
+      <c r="E18" s="8">
+        <v>117.86609792709299</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8">
+        <v>127.85326552391</v>
+      </c>
+      <c r="H18" s="8">
+        <f>G18/C18</f>
+        <v>1.1680094354772421</v>
+      </c>
+      <c r="I18" s="8">
+        <f t="shared" si="2"/>
+        <v>9.6464185714720116</v>
+      </c>
+      <c r="J18" s="8">
+        <f>I18/D18</f>
+        <v>1.1478953164041119</v>
+      </c>
+      <c r="K18" s="8">
+        <v>137.49968409538201</v>
+      </c>
+      <c r="L18" s="8">
+        <f>K18/E18</f>
+        <v>1.1665753470555504</v>
+      </c>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8">
+        <v>155.35111451148899</v>
+      </c>
+      <c r="O18" s="8">
+        <f>N18/C18</f>
+        <v>1.4192173099199501</v>
+      </c>
+      <c r="P18" s="8">
+        <f t="shared" si="6"/>
+        <v>10.069684505463016</v>
+      </c>
+      <c r="Q18" s="8">
+        <f>P18/D18</f>
+        <v>1.1982627123056921</v>
+      </c>
+      <c r="R18" s="8">
+        <v>165.420799016952</v>
+      </c>
+      <c r="S18" s="8">
+        <f>R18/E18</f>
+        <v>1.4034637773388778</v>
+      </c>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+    </row>
+    <row r="19" spans="1:21" ht="15.75">
+      <c r="A19" s="15"/>
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="8">
+        <v>102.343473911285</v>
+      </c>
+      <c r="D19" s="8">
+        <f t="shared" si="0"/>
+        <v>8.9783523082730028</v>
+      </c>
+      <c r="E19" s="8">
+        <v>111.32182621955801</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8">
+        <v>131.21943664550699</v>
+      </c>
+      <c r="H19" s="8">
+        <f>G19/C19</f>
+        <v>1.2821475725873124</v>
+      </c>
+      <c r="I19" s="8">
+        <f t="shared" si="2"/>
+        <v>10.251653671265018</v>
+      </c>
+      <c r="J19" s="8">
+        <f>I19/D19</f>
+        <v>1.1418190464433819</v>
+      </c>
+      <c r="K19" s="8">
+        <v>141.47109031677201</v>
+      </c>
+      <c r="L19" s="8">
+        <f>K19/E19</f>
+        <v>1.2708297655641325</v>
+      </c>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8">
+        <v>160.096146106719</v>
+      </c>
+      <c r="O19" s="8">
+        <f>N19/C19</f>
+        <v>1.5643024414580269</v>
+      </c>
+      <c r="P19" s="8">
+        <f t="shared" si="6"/>
+        <v>9.9259154796610005</v>
+      </c>
+      <c r="Q19" s="8">
+        <f>P19/D19</f>
+        <v>1.1055386488359202</v>
+      </c>
+      <c r="R19" s="8">
+        <v>170.02206158638</v>
+      </c>
+      <c r="S19" s="8">
+        <f>R19/E19</f>
+        <v>1.5273021235840005</v>
+      </c>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+    </row>
+    <row r="20" spans="1:21" s="11" customFormat="1" ht="15.75">
+      <c r="A20" s="9"/>
+      <c r="B20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="10">
+        <f>AVERAGE(C16:C19)</f>
+        <v>112.1012846231455</v>
+      </c>
+      <c r="D20" s="10">
+        <f t="shared" ref="D20:S20" si="11">AVERAGE(D16:D19)</f>
+        <v>8.8323078155517543</v>
+      </c>
+      <c r="E20" s="10">
+        <f t="shared" si="11"/>
+        <v>120.93359243869725</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10">
+        <f t="shared" si="11"/>
+        <v>136.03594589233325</v>
+      </c>
+      <c r="H20" s="12">
+        <f>G20/C20</f>
+        <v>1.2135092505821825</v>
+      </c>
+      <c r="I20" s="10">
+        <f t="shared" si="11"/>
+        <v>9.980779826641264</v>
+      </c>
+      <c r="J20" s="12">
+        <f>I20/D20</f>
+        <v>1.1300307954697075</v>
+      </c>
+      <c r="K20" s="10">
+        <f t="shared" si="11"/>
+        <v>146.0167257189745</v>
+      </c>
+      <c r="L20" s="12">
+        <f>K20/E20</f>
+        <v>1.2074124548395617</v>
+      </c>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10">
+        <f t="shared" si="11"/>
+        <v>165.32362079620276</v>
+      </c>
+      <c r="O20" s="12">
+        <f>N20/C20</f>
+        <v>1.4747700827156129</v>
+      </c>
+      <c r="P20" s="10">
+        <f t="shared" si="11"/>
+        <v>9.8932110071185022</v>
+      </c>
+      <c r="Q20" s="12">
+        <f>P20/D20</f>
+        <v>1.1201161931538131</v>
+      </c>
+      <c r="R20" s="10">
+        <f>AVERAGE(R16:R19)</f>
+        <v>175.21683180332127</v>
+      </c>
+      <c r="S20" s="12">
+        <f>R20/E20</f>
+        <v>1.4488681620215729</v>
+      </c>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+    </row>
+    <row r="21" spans="1:21" ht="15.75">
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
+    </row>
+    <row r="22" spans="1:21" ht="15.75">
+      <c r="A22" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="8">
+        <v>155.11121892929</v>
+      </c>
+      <c r="D22" s="8">
+        <f t="shared" si="0"/>
+        <v>10.072481155395991</v>
+      </c>
+      <c r="E22" s="8">
+        <v>165.183700084686</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8">
+        <v>202.180891990661</v>
+      </c>
+      <c r="H22" s="8">
+        <f>G22/C22</f>
+        <v>1.3034575666820623</v>
+      </c>
+      <c r="I22" s="8">
+        <f t="shared" si="2"/>
+        <v>11.086788892746</v>
+      </c>
+      <c r="J22" s="8">
+        <f>I22/D22</f>
+        <v>1.1007008821065531</v>
+      </c>
+      <c r="K22" s="8">
+        <v>213.267680883407</v>
+      </c>
+      <c r="L22" s="8">
+        <f>K22/E22</f>
+        <v>1.2910939806655828</v>
+      </c>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8">
+        <v>252.24619936943</v>
+      </c>
+      <c r="O22" s="8">
+        <f>N22/C22</f>
+        <v>1.626227948633558</v>
+      </c>
+      <c r="P22" s="8">
+        <f t="shared" si="6"/>
+        <v>11.058322191237977</v>
+      </c>
+      <c r="Q22" s="8">
+        <f>P22/D22</f>
+        <v>1.0978746964757393</v>
+      </c>
+      <c r="R22" s="8">
+        <v>263.30452156066798</v>
+      </c>
+      <c r="S22" s="8">
+        <f>R22/E22</f>
+        <v>1.5940103135217194</v>
+      </c>
+      <c r="T22" s="7"/>
+      <c r="U22" s="7"/>
+    </row>
+    <row r="23" spans="1:21" ht="15.75">
+      <c r="A23" s="15"/>
+      <c r="B23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="8">
+        <v>130.421717643737</v>
+      </c>
+      <c r="D23" s="8">
+        <f t="shared" si="0"/>
+        <v>9.7629649639129923</v>
+      </c>
+      <c r="E23" s="8">
+        <v>140.18468260764999</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8">
+        <v>168.444113969802</v>
+      </c>
+      <c r="H23" s="8">
+        <f>G23/C23</f>
+        <v>1.2915342399486553</v>
+      </c>
+      <c r="I23" s="8">
+        <f t="shared" si="2"/>
+        <v>11.039766788483007</v>
+      </c>
+      <c r="J23" s="8">
+        <f>I23/D23</f>
+        <v>1.1307801297341</v>
+      </c>
+      <c r="K23" s="8">
+        <v>179.48388075828501</v>
+      </c>
+      <c r="L23" s="8">
+        <f>K23/E23</f>
+        <v>1.2803387461426576</v>
+      </c>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8">
+        <v>212.61090064048699</v>
+      </c>
+      <c r="O23" s="8">
+        <f>N23/C23</f>
+        <v>1.6301801914713305</v>
+      </c>
+      <c r="P23" s="8">
+        <f t="shared" si="6"/>
+        <v>10.656936645508011</v>
+      </c>
+      <c r="Q23" s="8">
+        <f>P23/D23</f>
+        <v>1.091567642094325</v>
+      </c>
+      <c r="R23" s="8">
+        <v>223.267837285995</v>
+      </c>
+      <c r="S23" s="8">
+        <f>R23/E23</f>
+        <v>1.5926692783610232</v>
+      </c>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+    </row>
+    <row r="24" spans="1:21" ht="15.75">
+      <c r="A24" s="15"/>
+      <c r="B24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="8">
+        <v>130.089377641677</v>
+      </c>
+      <c r="D24" s="8">
+        <f t="shared" si="0"/>
+        <v>9.2206494808199864</v>
+      </c>
+      <c r="E24" s="8">
+        <v>139.31002712249699</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8">
+        <v>166.95269131660399</v>
+      </c>
+      <c r="H24" s="8">
+        <f>G24/C24</f>
+        <v>1.2833691293109624</v>
+      </c>
+      <c r="I24" s="8">
+        <f t="shared" si="2"/>
+        <v>10.705965757370024</v>
+      </c>
+      <c r="J24" s="8">
+        <f>I24/D24</f>
+        <v>1.1610858627301326</v>
+      </c>
+      <c r="K24" s="8">
+        <v>177.65865707397401</v>
+      </c>
+      <c r="L24" s="8">
+        <f>K24/E24</f>
+        <v>1.2752754467397858</v>
+      </c>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8">
+        <v>210.11298155784601</v>
+      </c>
+      <c r="O24" s="8">
+        <f>N24/C24</f>
+        <v>1.6151432604788762</v>
+      </c>
+      <c r="P24" s="8">
+        <f t="shared" si="6"/>
+        <v>10.491855144499993</v>
+      </c>
+      <c r="Q24" s="8">
+        <f>P24/D24</f>
+        <v>1.1378650892569186</v>
+      </c>
+      <c r="R24" s="8">
+        <v>220.60483670234601</v>
+      </c>
+      <c r="S24" s="8">
+        <f>R24/E24</f>
+        <v>1.5835531817703654</v>
+      </c>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+    </row>
+    <row r="25" spans="1:21" ht="15.75">
+      <c r="A25" s="15"/>
+      <c r="B25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="8">
+        <v>134.866724014282</v>
+      </c>
+      <c r="D25" s="8">
+        <f t="shared" si="0"/>
+        <v>9.6382646560670082</v>
+      </c>
+      <c r="E25" s="8">
+        <v>144.50498867034901</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8">
+        <v>174.79175829887299</v>
+      </c>
+      <c r="H25" s="8">
+        <f>G25/C25</f>
+        <v>1.2960332474626064</v>
+      </c>
+      <c r="I25" s="8">
+        <f t="shared" si="2"/>
+        <v>11.083686113357999</v>
+      </c>
+      <c r="J25" s="8">
+        <f>I25/D25</f>
+        <v>1.1499669814919575</v>
+      </c>
+      <c r="K25" s="8">
+        <v>185.87544441223099</v>
+      </c>
+      <c r="L25" s="8">
+        <f>K25/E25</f>
+        <v>1.2862908479669033</v>
+      </c>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8">
+        <v>221.47290802001899</v>
+      </c>
+      <c r="O25" s="8">
+        <f>N25/C25</f>
+        <v>1.6421612494759319</v>
+      </c>
+      <c r="P25" s="8">
+        <f t="shared" si="6"/>
+        <v>10.771953582764013</v>
+      </c>
+      <c r="Q25" s="8">
+        <f>P25/D25</f>
+        <v>1.1176237597899308</v>
+      </c>
+      <c r="R25" s="8">
+        <v>232.244861602783</v>
+      </c>
+      <c r="S25" s="8">
+        <f>R25/E25</f>
+        <v>1.6071753905506332</v>
+      </c>
+      <c r="T25" s="7"/>
+      <c r="U25" s="7"/>
+    </row>
+    <row r="26" spans="1:21" s="11" customFormat="1" ht="15.75">
+      <c r="A26" s="9"/>
+      <c r="B26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="10">
+        <f>AVERAGE(C22:C25)</f>
+        <v>137.62225955724648</v>
+      </c>
+      <c r="D26" s="10">
+        <f t="shared" ref="D26:S26" si="12">AVERAGE(D22:D25)</f>
+        <v>9.6735900640489945</v>
+      </c>
+      <c r="E26" s="10">
+        <f t="shared" si="12"/>
+        <v>147.2958496212955</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10">
+        <f t="shared" si="12"/>
+        <v>178.09236389398501</v>
+      </c>
+      <c r="H26" s="12">
+        <f>G26/C26</f>
+        <v>1.294066559195711</v>
+      </c>
+      <c r="I26" s="10">
+        <f t="shared" si="12"/>
+        <v>10.979051887989257</v>
+      </c>
+      <c r="J26" s="12">
+        <f>I26/D26</f>
+        <v>1.1349511210726089</v>
+      </c>
+      <c r="K26" s="10">
+        <f t="shared" si="12"/>
+        <v>189.07141578197425</v>
+      </c>
+      <c r="L26" s="12">
+        <f>K26/E26</f>
+        <v>1.283616722861409</v>
+      </c>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10">
+        <f t="shared" si="12"/>
+        <v>224.11074739694547</v>
+      </c>
+      <c r="O26" s="12">
+        <f>N26/C26</f>
+        <v>1.6284483928540827</v>
+      </c>
+      <c r="P26" s="10">
+        <f t="shared" si="12"/>
+        <v>10.744766891002499</v>
+      </c>
+      <c r="Q26" s="12">
+        <f>P26/D26</f>
+        <v>1.1107320880729104</v>
+      </c>
+      <c r="R26" s="10">
+        <f>AVERAGE(R22:R25)</f>
+        <v>234.85551428794798</v>
+      </c>
+      <c r="S26" s="12">
+        <f>R26/E26</f>
+        <v>1.5944476025072836</v>
+      </c>
+      <c r="T26" s="13"/>
+      <c r="U26" s="13"/>
+    </row>
+    <row r="27" spans="1:21" ht="15.75">
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="8"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
+    </row>
+    <row r="28" spans="1:21" ht="15" customHeight="1">
+      <c r="A28" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="8">
+        <v>102.81528592109601</v>
+      </c>
+      <c r="D28" s="8">
+        <f t="shared" si="0"/>
+        <v>89.954488992690983</v>
+      </c>
+      <c r="E28" s="8">
+        <v>192.76977491378699</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8">
+        <v>117.203608274459</v>
+      </c>
+      <c r="H28" s="8">
+        <f>G28/C28</f>
+        <v>1.1399434162387594</v>
+      </c>
+      <c r="I28" s="8">
+        <f t="shared" si="2"/>
+        <v>96.960754394532003</v>
+      </c>
+      <c r="J28" s="8">
+        <f>I28/D28</f>
+        <v>1.0778867789734239</v>
+      </c>
+      <c r="K28" s="8">
+        <v>214.164362668991</v>
+      </c>
+      <c r="L28" s="8">
+        <f>K28/E28</f>
+        <v>1.1109851778618944</v>
+      </c>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8">
+        <v>148.52965426444999</v>
+      </c>
+      <c r="O28" s="8">
+        <f>N28/C28</f>
+        <v>1.4446261850444764</v>
+      </c>
+      <c r="P28" s="8">
+        <f t="shared" si="6"/>
+        <v>87.823757410049012</v>
+      </c>
+      <c r="Q28" s="8">
+        <f>P28/D28</f>
+        <v>0.97631322676053334</v>
+      </c>
+      <c r="R28" s="8">
+        <v>236.353411674499</v>
+      </c>
+      <c r="S28" s="8">
+        <f>R28/E28</f>
+        <v>1.2260916514541973</v>
+      </c>
+      <c r="T28" s="7"/>
+      <c r="U28" s="7"/>
+    </row>
+    <row r="29" spans="1:21" ht="15.75">
+      <c r="A29" s="15"/>
+      <c r="B29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="8">
+        <v>99.240627050399695</v>
+      </c>
+      <c r="D29" s="8">
+        <f t="shared" si="0"/>
+        <v>89.586415767669308</v>
+      </c>
+      <c r="E29" s="8">
+        <v>188.827042818069</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8">
+        <v>101.458420991897</v>
+      </c>
+      <c r="H29" s="8">
+        <f>G29/C29</f>
+        <v>1.0223476413583219</v>
+      </c>
+      <c r="I29" s="8">
+        <f t="shared" si="2"/>
+        <v>95.646151304245009</v>
+      </c>
+      <c r="J29" s="8">
+        <f>I29/D29</f>
+        <v>1.0676412320400319</v>
+      </c>
+      <c r="K29" s="8">
+        <v>197.10457229614201</v>
+      </c>
+      <c r="L29" s="8">
+        <f>K29/E29</f>
+        <v>1.0438365678694033</v>
+      </c>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8">
+        <v>128.55381655693</v>
+      </c>
+      <c r="O29" s="8">
+        <f>N29/C29</f>
+        <v>1.2953748920957895</v>
+      </c>
+      <c r="P29" s="8">
+        <f t="shared" si="6"/>
+        <v>93.039846420288001</v>
+      </c>
+      <c r="Q29" s="8">
+        <f>P29/D29</f>
+        <v>1.0385485971620376</v>
+      </c>
+      <c r="R29" s="8">
+        <v>221.593662977218</v>
+      </c>
+      <c r="S29" s="8">
+        <f>R29/E29</f>
+        <v>1.1735271583462701</v>
+      </c>
+      <c r="T29" s="7"/>
+      <c r="U29" s="7"/>
+    </row>
+    <row r="30" spans="1:21" ht="35.1" customHeight="1">
+      <c r="A30" s="15"/>
+      <c r="B30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="8">
+        <v>93.270155906677203</v>
+      </c>
+      <c r="D30" s="8">
+        <f t="shared" si="0"/>
+        <v>81.656078338622805</v>
+      </c>
+      <c r="E30" s="8">
+        <v>174.92623424530001</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8">
+        <v>109.42152214050201</v>
+      </c>
+      <c r="H30" s="8">
+        <f>G30/C30</f>
+        <v>1.1731675698064157</v>
+      </c>
+      <c r="I30" s="8">
+        <f t="shared" si="2"/>
+        <v>92.089767694473991</v>
+      </c>
+      <c r="J30" s="8">
+        <f>I30/D30</f>
+        <v>1.1277760280451299</v>
+      </c>
+      <c r="K30" s="8">
+        <v>201.511289834976</v>
+      </c>
+      <c r="L30" s="8">
+        <f>K30/E30</f>
+        <v>1.1519786652035029</v>
+      </c>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8">
+        <v>139.34928870201099</v>
+      </c>
+      <c r="O30" s="8">
+        <f>N30/C30</f>
+        <v>1.4940394100063361</v>
+      </c>
+      <c r="P30" s="8">
+        <f t="shared" si="6"/>
+        <v>84.376674413681002</v>
+      </c>
+      <c r="Q30" s="8">
+        <f>P30/D30</f>
+        <v>1.0333177410722083</v>
+      </c>
+      <c r="R30" s="8">
+        <v>223.725963115692</v>
+      </c>
+      <c r="S30" s="8">
+        <f>R30/E30</f>
+        <v>1.2789731859313902</v>
+      </c>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+    </row>
+    <row r="31" spans="1:21" s="11" customFormat="1" ht="15.75">
+      <c r="A31" s="5"/>
+      <c r="B31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="10">
+        <f>AVERAGE(C28:C30)</f>
+        <v>98.442022959390968</v>
+      </c>
+      <c r="D31" s="10">
+        <f t="shared" ref="D31:S31" si="13">AVERAGE(D28:D30)</f>
+        <v>87.065661032994356</v>
+      </c>
+      <c r="E31" s="10">
+        <f t="shared" si="13"/>
+        <v>185.50768399238532</v>
+      </c>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10">
+        <f t="shared" si="13"/>
+        <v>109.36118380228601</v>
+      </c>
+      <c r="H31" s="12">
+        <f>G31/C31</f>
+        <v>1.1109197120766137</v>
+      </c>
+      <c r="I31" s="10">
+        <f t="shared" si="13"/>
+        <v>94.898891131083658</v>
+      </c>
+      <c r="J31" s="12">
+        <f>I31/D31</f>
+        <v>1.0899692255839053</v>
+      </c>
+      <c r="K31" s="10">
+        <f t="shared" si="13"/>
+        <v>204.26007493336965</v>
+      </c>
+      <c r="L31" s="12">
+        <f>K31/E31</f>
+        <v>1.1010868689501512</v>
+      </c>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10">
+        <f t="shared" si="13"/>
+        <v>138.81091984113033</v>
+      </c>
+      <c r="O31" s="12">
+        <f>N31/C31</f>
+        <v>1.4100778881635969</v>
+      </c>
+      <c r="P31" s="10">
+        <f t="shared" si="13"/>
+        <v>88.413426081339324</v>
+      </c>
+      <c r="Q31" s="12">
+        <f>P31/D31</f>
+        <v>1.0154798692429869</v>
+      </c>
+      <c r="R31" s="10">
+        <f>AVERAGE(R28:R30)</f>
+        <v>227.22434592246967</v>
+      </c>
+      <c r="S31" s="12">
+        <f>R31/E31</f>
+        <v>1.2248783502240086</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="A32" s="5"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:17" ht="29.25">
+      <c r="A33" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="H33" s="13">
+        <f>AVERAGE(H9,H14,H20,H26,H31)</f>
+        <v>1.2968155350436281</v>
+      </c>
+      <c r="I33" s="11"/>
+      <c r="J33" s="13">
+        <f>AVERAGE(J9,J14,J20,J26,J31)</f>
+        <v>1.1527243559885647</v>
+      </c>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="13">
+        <f>AVERAGE(O9,O14,O20,O26,O31)</f>
+        <v>1.5877516456291267</v>
+      </c>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="13">
+        <f>AVERAGE(Q9,Q14,Q20,Q26,Q31)</f>
+        <v>1.1378461759754892</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="A34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="K1:U1"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="N3:R3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E10:G10 K10 R10 M10:N10">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>